<commit_message>
added bill settlement promotion 121 and changes in sales invoice estimate for thetestcases
</commit_message>
<xml_diff>
--- a/src/test/java/datafiles/Barcodescan.xlsx
+++ b/src/test/java/datafiles/Barcodescan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Barcode_promotion_121</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>Barcode_promotion_123</t>
+  </si>
+  <si>
+    <t>ś</t>
   </si>
   <si>
     <t>Barcode_promotion_124</t>
@@ -42,10 +45,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -61,6 +64,67 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -69,7 +133,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -77,15 +141,23 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -99,100 +171,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -220,25 +223,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -250,151 +397,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -417,38 +420,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -464,11 +437,24 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -489,15 +475,30 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -505,9 +506,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -516,152 +519,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -672,9 +675,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -999,13 +999,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A34"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="29.7142857142857" customWidth="1"/>
   </cols>
@@ -1066,7 +1066,7 @@
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="5">
+      <c r="A12" s="4">
         <v>172210801</v>
       </c>
     </row>
@@ -1080,9 +1080,12 @@
         <v>159433876</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:5">
       <c r="A15" s="4">
         <v>221664314</v>
+      </c>
+      <c r="E15" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:1">
@@ -1092,7 +1095,7 @@
     </row>
     <row r="17" ht="15.75" spans="1:1">
       <c r="A17" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:1">
@@ -1132,7 +1135,7 @@
     </row>
     <row r="25" ht="15.75" spans="1:1">
       <c r="A25" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:1">
@@ -1157,7 +1160,7 @@
     </row>
     <row r="30" ht="15.75" spans="1:1">
       <c r="A30" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:1">

</xml_diff>